<commit_message>
Correzione data rilascio revisione 00
</commit_message>
<xml_diff>
--- a/Versionamento/Indice versioni.xlsx
+++ b/Versionamento/Indice versioni.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gessica.dilenardo\Documents\Power BI\Elaborati\BI_Magazzino_Anagrafica_Articoli\Versionamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29365860-0B98-4A0E-A175-7EF3C4B57036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABB7C99-4A3E-4170-9986-DE8DECA789C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-270" windowWidth="29040" windowHeight="15720" xr2:uid="{E8661EE8-0424-44C1-8E9C-476E929CF0A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E8661EE8-0424-44C1-8E9C-476E929CF0A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>n° versione</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>0.0</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>Inserimento versione progetto</t>
   </si>
 </sst>
 </file>
@@ -118,8 +124,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DA6D639-3982-49E4-9273-EDF18E8E0296}" name="Indice_versioni" displayName="Indice_versioni" ref="A1:D2" totalsRowShown="0">
-  <autoFilter ref="A1:D2" xr:uid="{3DA6D639-3982-49E4-9273-EDF18E8E0296}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DA6D639-3982-49E4-9273-EDF18E8E0296}" name="Indice_versioni" displayName="Indice_versioni" ref="A1:D3" totalsRowShown="0">
+  <autoFilter ref="A1:D3" xr:uid="{3DA6D639-3982-49E4-9273-EDF18E8E0296}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{DF868F52-5EA1-4396-A148-08152EED9F75}" name="n° versione"/>
     <tableColumn id="2" xr3:uid="{4C524CEA-5424-4979-BFA7-A9FA81F03901}" name="Modifiche" dataDxfId="1"/>
@@ -427,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F82909-EF29-41C9-80BE-D5671978DDB6}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,7 +472,18 @@
         <v>45630</v>
       </c>
       <c r="D2" s="1">
-        <v>45656</v>
+        <v>45626</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45642</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correzione versione errata nella data
</commit_message>
<xml_diff>
--- a/Versionamento/Indice versioni.xlsx
+++ b/Versionamento/Indice versioni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gessica.dilenardo\Documents\Power BI\Elaborati\BI_Magazzino_Anagrafica_Articoli\Versionamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDE24E6-1453-43C4-BAAA-8E27474662AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839DEDBD-64D5-414C-98B0-8983584228BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-270" windowWidth="29040" windowHeight="15720" xr2:uid="{E8661EE8-0424-44C1-8E9C-476E929CF0A3}"/>
   </bookViews>
@@ -442,7 +442,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +503,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="1">
-        <v>45305</v>
+        <v>45671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ver 0.3 dev sviluppo pagina per sistemazione anagrafica artcoli
Inserita pagina movimentazione articoli, aggiunte tabelle mmov, mcau, s/conti, ordini di acquisto per permettere analizzare dati in funzione del progetto di sistemazione delle anagrafiche articoli industriali e commerciali
</commit_message>
<xml_diff>
--- a/Versionamento/Indice versioni.xlsx
+++ b/Versionamento/Indice versioni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gessica.dilenardo\Documents\Power BI\Elaborati\BI_Magazzino_Anagrafica_Articoli\Versionamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78222FF1-025B-4EF8-ABAC-430B575361F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AC5835-CE62-4C25-BB71-AC709DFB9A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-270" windowWidth="29040" windowHeight="15720" xr2:uid="{E8661EE8-0424-44C1-8E9C-476E929CF0A3}"/>
   </bookViews>
@@ -448,7 +448,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,7 +512,7 @@
         <v>45671</v>
       </c>
       <c r="D4" s="1">
-        <v>45677</v>
+        <v>45676</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>